<commit_message>
new ephochs are executed
</commit_message>
<xml_diff>
--- a/data/model_performance.xlsx
+++ b/data/model_performance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1082,6 +1082,80 @@
         <v>0.9250701773268788</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2023-10-31-23-26-54</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="C18" t="n">
+        <v>50</v>
+      </c>
+      <c r="D18" t="n">
+        <v>5</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" t="n">
+        <v>64</v>
+      </c>
+      <c r="G18" t="n">
+        <v>106.328522121165</v>
+      </c>
+      <c r="H18" t="n">
+        <v>19700.85450868611</v>
+      </c>
+      <c r="I18" t="n">
+        <v>140.3597325043266</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.1999540328979492</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.6642365604186027</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2023-11-01-19-58-13</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="C19" t="n">
+        <v>50</v>
+      </c>
+      <c r="D19" t="n">
+        <v>20</v>
+      </c>
+      <c r="E19" t="n">
+        <v>50</v>
+      </c>
+      <c r="F19" t="n">
+        <v>64</v>
+      </c>
+      <c r="G19" t="n">
+        <v>13.46708038330078</v>
+      </c>
+      <c r="H19" t="n">
+        <v>298.8550831759035</v>
+      </c>
+      <c r="I19" t="n">
+        <v>17.28742557976472</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.003033227985724807</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.9949112311223018</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>